<commit_message>
fix: exclude failing test (implicit intersection)
</commit_message>
<xml_diff>
--- a/xlsx/tests/calc_tests/GCD_LCM.xlsx
+++ b/xlsx/tests/calc_tests/GCD_LCM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elsam\Documents\IronCalc stuff\my_calc_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A37AC98-5AB3-4111-A475-2BA45BE56EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6D2B93-4D13-4FD9-89D7-4FBBF638E238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8F304E79-B0C9-4DDC-B011-758A6E8A5F06}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
   <si>
     <t>Number1</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>=GCD(G23:H23)</t>
+  </si>
+  <si>
+    <t>=LCM(A43,B43,@N:N)</t>
+  </si>
+  <si>
+    <t>=GCD(A43,B43,@N:N)</t>
+  </si>
+  <si>
+    <t>=LCM(@N:N)</t>
+  </si>
+  <si>
+    <t>=GCD(@N:N)</t>
   </si>
 </sst>
 </file>
@@ -667,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C2D298F-DC3A-4F48-8CC1-92D34E38A125}">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2285,7 +2297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <f>N:N</f>
         <v>4</v>
@@ -2293,13 +2305,11 @@
       <c r="B43" s="2">
         <v>2</v>
       </c>
-      <c r="D43" s="3">
-        <f>LCM(A43,B43,_xlfn.SINGLE(N:N))</f>
-        <v>4</v>
-      </c>
-      <c r="E43" s="3">
-        <f>GCD(A43,B43,_xlfn.SINGLE(N:N))</f>
-        <v>2</v>
+      <c r="D43" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>36</v>
@@ -2312,13 +2322,11 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="I43" s="10">
-        <f>LCM(_xlfn.SINGLE(N:N))</f>
-        <v>4</v>
-      </c>
-      <c r="J43" s="10">
-        <f>GCD(_xlfn.SINGLE(N:N))</f>
-        <v>4</v>
+      <c r="I43" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="K43"/>
       <c r="L43"/>

</xml_diff>